<commit_message>
some UI changes and Type Into fix
</commit_message>
<xml_diff>
--- a/Excel files/cars parameters.xlsx
+++ b/Excel files/cars parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <x:si>
     <x:t>CarName</x:t>
   </x:si>
@@ -25,78 +25,48 @@
     <x:t>CarPrice</x:t>
   </x:si>
   <x:si>
+    <x:t>Tesla Model X I, 6 мест</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/108444907</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tesla Model X I, 7 мест</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/105562879</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/109631463</x:t>
+  </x:si>
+  <x:si>
     <x:t>Tesla Model X I · Рестайлинг, 6 мест</x:t>
   </x:si>
   <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110352839</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110336741</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110405797</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/109384939</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tesla Model X I · Рестайлинг</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/109287918</x:t>
+    <x:t>https://cars.av.by/tesla/model-x/109872261</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/109578074</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/110405384</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/110121889</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/109905270</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/110405848</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/106217374</x:t>
   </x:si>
   <x:si>
     <x:t>Tesla Model X I</x:t>
   </x:si>
   <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/103694589</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tesla Model X I, 6 мест</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/104400486</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/107287543</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/108444907</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tesla Model X I, 7 мест</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/107203117</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/105562879</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/109631463</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/109872261</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/109578074</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110405384</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110121889</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/109905270</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110405848</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/106217374</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://cars.av.by/tesla/model-x/100804369</x:t>
   </x:si>
   <x:si>
@@ -209,30 +179,6 @@
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/tesla/model-x/108439391</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110225839</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110297676</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110432057</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/104088131</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/108658646</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/107709262</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/109699771</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/110441062</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -583,7 +529,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C66"/>
+  <x:dimension ref="A1:C49"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -608,18 +554,18 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
-        <x:v>388948</x:v>
+        <x:v>223164</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
-        <x:v>315622</x:v>
+        <x:v>216788</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
@@ -627,87 +573,87 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
-        <x:v>315622</x:v>
+        <x:v>207227</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C5" s="0" t="n">
-        <x:v>302870</x:v>
+        <x:v>207227</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C6" s="0" t="n">
-        <x:v>286929</x:v>
+        <x:v>192880</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C7" s="0" t="n">
-        <x:v>256642</x:v>
+        <x:v>191286</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
       <x:c r="C8" s="0" t="n">
-        <x:v>253135</x:v>
+        <x:v>191286</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C9" s="0" t="n">
-        <x:v>251860</x:v>
+        <x:v>191283</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C10" s="0" t="n">
-        <x:v>223164</x:v>
+        <x:v>191254</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C11" s="0" t="n">
-        <x:v>219976</x:v>
+        <x:v>190967</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
@@ -715,21 +661,21 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C12" s="0" t="n">
-        <x:v>216788</x:v>
+        <x:v>188098</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="A13" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C13" s="0" t="n">
-        <x:v>207227</x:v>
+        <x:v>187141</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
@@ -737,10 +683,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C14" s="0" t="n">
-        <x:v>207227</x:v>
+        <x:v>159373</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
@@ -748,571 +694,384 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C15" s="0" t="n">
-        <x:v>192880</x:v>
+        <x:v>159086</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C16" s="0" t="n">
-        <x:v>191286</x:v>
+        <x:v>156217</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="A17" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C17" s="0" t="n">
-        <x:v>191286</x:v>
+        <x:v>156214</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C18" s="0" t="n">
-        <x:v>191283</x:v>
+        <x:v>146621</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C19" s="0" t="n">
-        <x:v>191254</x:v>
+        <x:v>146334</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="A20" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C20" s="0" t="n">
-        <x:v>190967</x:v>
+        <x:v>143465</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C21" s="0" t="n">
-        <x:v>188098</x:v>
+        <x:v>143465</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="A22" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C22" s="0" t="n">
-        <x:v>187141</x:v>
+        <x:v>143465</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
       <x:c r="A23" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C23" s="0" t="n">
-        <x:v>159373</x:v>
+        <x:v>141870</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
       <x:c r="A24" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C24" s="0" t="n">
-        <x:v>159086</x:v>
+        <x:v>137088</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
       <x:c r="A25" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C25" s="0" t="n">
-        <x:v>156217</x:v>
+        <x:v>135494</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3">
       <x:c r="A26" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C26" s="0" t="n">
-        <x:v>156214</x:v>
+        <x:v>133581</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
       <x:c r="A27" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C27" s="0" t="n">
-        <x:v>146621</x:v>
+        <x:v>132306</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3">
       <x:c r="A28" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C28" s="0" t="n">
-        <x:v>146334</x:v>
+        <x:v>131031</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="A29" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C29" s="0" t="n">
-        <x:v>143465</x:v>
+        <x:v>127524</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="A30" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C30" s="0" t="n">
-        <x:v>143465</x:v>
+        <x:v>127492</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3">
       <x:c r="A31" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C31" s="0" t="n">
-        <x:v>143465</x:v>
+        <x:v>125930</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="A32" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C32" s="0" t="n">
-        <x:v>141870</x:v>
+        <x:v>122742</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">
       <x:c r="A33" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C33" s="0" t="n">
-        <x:v>137088</x:v>
+        <x:v>122742</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:3">
       <x:c r="A34" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C34" s="0" t="n">
-        <x:v>135494</x:v>
+        <x:v>120829</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="A35" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C35" s="0" t="n">
-        <x:v>133581</x:v>
+        <x:v>119554</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:3">
       <x:c r="A36" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C36" s="0" t="n">
-        <x:v>132306</x:v>
+        <x:v>119554</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="A37" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C37" s="0" t="n">
-        <x:v>131031</x:v>
+        <x:v>117957</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:3">
       <x:c r="A38" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C38" s="0" t="n">
-        <x:v>127524</x:v>
+        <x:v>114453</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:3">
       <x:c r="A39" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C39" s="0" t="n">
-        <x:v>127492</x:v>
+        <x:v>111902</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:3">
       <x:c r="A40" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C40" s="0" t="n">
-        <x:v>125930</x:v>
+        <x:v>111584</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:3">
       <x:c r="A41" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C41" s="0" t="n">
-        <x:v>122742</x:v>
+        <x:v>111584</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:3">
       <x:c r="A42" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C42" s="0" t="n">
-        <x:v>122742</x:v>
+        <x:v>111265</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:3">
       <x:c r="A43" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C43" s="0" t="n">
-        <x:v>120829</x:v>
+        <x:v>111265</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:3">
       <x:c r="A44" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C44" s="0" t="n">
-        <x:v>119554</x:v>
+        <x:v>109989</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:3">
       <x:c r="A45" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C45" s="0" t="n">
-        <x:v>119554</x:v>
+        <x:v>108392</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:3">
       <x:c r="A46" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C46" s="0" t="n">
-        <x:v>117957</x:v>
+        <x:v>103613</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:3">
       <x:c r="A47" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C47" s="0" t="n">
-        <x:v>114453</x:v>
+        <x:v>102016</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:3">
       <x:c r="A48" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C48" s="0" t="n">
-        <x:v>111902</x:v>
+        <x:v>101700</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:3">
       <x:c r="A49" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C49" s="0" t="n">
-        <x:v>111584</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="50" spans="1:3">
-      <x:c r="A50" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B50" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="C50" s="0" t="n">
-        <x:v>111584</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="51" spans="1:3">
-      <x:c r="A51" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B51" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="C51" s="0" t="n">
-        <x:v>111265</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="52" spans="1:3">
-      <x:c r="A52" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B52" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="C52" s="0" t="n">
-        <x:v>111265</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="53" spans="1:3">
-      <x:c r="A53" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B53" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="C53" s="0" t="n">
-        <x:v>109989</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="54" spans="1:3">
-      <x:c r="A54" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B54" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="C54" s="0" t="n">
-        <x:v>108392</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="55" spans="1:3">
-      <x:c r="A55" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B55" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="C55" s="0" t="n">
-        <x:v>103613</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="56" spans="1:3">
-      <x:c r="A56" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B56" s="0" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="C56" s="0" t="n">
-        <x:v>102016</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="57" spans="1:3">
-      <x:c r="A57" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B57" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="C57" s="0" t="n">
-        <x:v>101700</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="58" spans="1:3">
-      <x:c r="A58" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B58" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="C58" s="0" t="n">
         <x:v>100425</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="59" spans="1:3">
-      <x:c r="A59" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B59" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="C59" s="0" t="n">
-        <x:v>98831</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="60" spans="1:3">
-      <x:c r="A60" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B60" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="C60" s="0" t="n">
-        <x:v>98672</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="61" spans="1:3">
-      <x:c r="A61" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B61" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="C61" s="0" t="n">
-        <x:v>98512</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="62" spans="1:3">
-      <x:c r="A62" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B62" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="C62" s="0" t="n">
-        <x:v>95640</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="63" spans="1:3">
-      <x:c r="A63" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B63" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C63" s="0" t="n">
-        <x:v>95324</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="64" spans="1:3">
-      <x:c r="A64" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B64" s="0" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C64" s="0" t="n">
-        <x:v>92455</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="65" spans="1:3">
-      <x:c r="A65" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B65" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="C65" s="0" t="n">
-        <x:v>90861</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="66" spans="1:3">
-      <x:c r="A66" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B66" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="C66" s="0" t="n">
-        <x:v>87673</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
UI result changes, add hyperlinks
</commit_message>
<xml_diff>
--- a/Excel files/cars parameters.xlsx
+++ b/Excel files/cars parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <x:si>
     <x:t>CarName</x:t>
   </x:si>
@@ -25,9 +25,33 @@
     <x:t>CarPrice</x:t>
   </x:si>
   <x:si>
+    <x:t>Tesla Model X I · Рестайлинг</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/110458856</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/109287918</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/109256994</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tesla Model X I</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/103694589</x:t>
+  </x:si>
+  <x:si>
     <x:t>Tesla Model X I, 6 мест</x:t>
   </x:si>
   <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/104400486</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/107287543</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://cars.av.by/tesla/model-x/108444907</x:t>
   </x:si>
   <x:si>
@@ -64,9 +88,6 @@
     <x:t>https://cars.av.by/tesla/model-x/106217374</x:t>
   </x:si>
   <x:si>
-    <x:t>Tesla Model X I</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://cars.av.by/tesla/model-x/100804369</x:t>
   </x:si>
   <x:si>
@@ -163,9 +184,6 @@
     <x:t>https://cars.av.by/tesla/model-x/106319825</x:t>
   </x:si>
   <x:si>
-    <x:t>https://cars.av.by/tesla/model-x/106447119</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://cars.av.by/tesla/model-x/110406206</x:t>
   </x:si>
   <x:si>
@@ -179,6 +197,30 @@
   </x:si>
   <x:si>
     <x:t>https://cars.av.by/tesla/model-x/108439391</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/110225839</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/110297676</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/110432057</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/104088131</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/108658646</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/107709262</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/109699771</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cars.av.by/tesla/model-x/110441062</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -529,7 +571,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C49"/>
+  <x:dimension ref="A1:C62"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -554,18 +596,18 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
-        <x:v>223164</x:v>
+        <x:v>282147</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
       <x:c r="C3" s="0" t="n">
-        <x:v>216788</x:v>
+        <x:v>270985</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
@@ -573,505 +615,648 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
-        <x:v>207227</x:v>
+        <x:v>270670</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="C5" s="0" t="n">
-        <x:v>207227</x:v>
+        <x:v>256642</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C6" s="0" t="n">
-        <x:v>192880</x:v>
+        <x:v>253135</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C7" s="0" t="n">
-        <x:v>191286</x:v>
+        <x:v>251860</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="C8" s="0" t="n">
-        <x:v>191286</x:v>
+        <x:v>223164</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C9" s="0" t="n">
-        <x:v>191283</x:v>
+        <x:v>216788</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C10" s="0" t="n">
-        <x:v>191254</x:v>
+        <x:v>207227</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C11" s="0" t="n">
-        <x:v>190967</x:v>
+        <x:v>207227</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
       <x:c r="A12" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C12" s="0" t="n">
-        <x:v>188098</x:v>
+        <x:v>192880</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="A13" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C13" s="0" t="n">
-        <x:v>187141</x:v>
+        <x:v>191286</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
       <x:c r="A14" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C14" s="0" t="n">
-        <x:v>159373</x:v>
+        <x:v>191286</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="A15" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C15" s="0" t="n">
-        <x:v>159086</x:v>
+        <x:v>191283</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C16" s="0" t="n">
-        <x:v>156217</x:v>
+        <x:v>191254</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="A17" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C17" s="0" t="n">
-        <x:v>156214</x:v>
+        <x:v>190967</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C18" s="0" t="n">
-        <x:v>146621</x:v>
+        <x:v>188098</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C19" s="0" t="n">
-        <x:v>146334</x:v>
+        <x:v>187141</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="A20" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C20" s="0" t="n">
-        <x:v>143465</x:v>
+        <x:v>159373</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C21" s="0" t="n">
-        <x:v>143465</x:v>
+        <x:v>159086</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="A22" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C22" s="0" t="n">
-        <x:v>143465</x:v>
+        <x:v>156217</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
       <x:c r="A23" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C23" s="0" t="n">
-        <x:v>141870</x:v>
+        <x:v>156214</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
       <x:c r="A24" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C24" s="0" t="n">
-        <x:v>137088</x:v>
+        <x:v>146621</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
       <x:c r="A25" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C25" s="0" t="n">
-        <x:v>135494</x:v>
+        <x:v>146334</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3">
       <x:c r="A26" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C26" s="0" t="n">
-        <x:v>133581</x:v>
+        <x:v>143465</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
       <x:c r="A27" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C27" s="0" t="n">
-        <x:v>132306</x:v>
+        <x:v>143465</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3">
       <x:c r="A28" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C28" s="0" t="n">
-        <x:v>131031</x:v>
+        <x:v>143465</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="A29" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C29" s="0" t="n">
-        <x:v>127524</x:v>
+        <x:v>141870</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="A30" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C30" s="0" t="n">
-        <x:v>127492</x:v>
+        <x:v>137088</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3">
       <x:c r="A31" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C31" s="0" t="n">
-        <x:v>125930</x:v>
+        <x:v>135494</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="A32" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C32" s="0" t="n">
-        <x:v>122742</x:v>
+        <x:v>133581</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">
       <x:c r="A33" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C33" s="0" t="n">
-        <x:v>122742</x:v>
+        <x:v>132306</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:3">
       <x:c r="A34" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C34" s="0" t="n">
-        <x:v>120829</x:v>
+        <x:v>131031</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="A35" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C35" s="0" t="n">
-        <x:v>119554</x:v>
+        <x:v>127524</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:3">
       <x:c r="A36" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C36" s="0" t="n">
-        <x:v>119554</x:v>
+        <x:v>127492</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="A37" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C37" s="0" t="n">
-        <x:v>117957</x:v>
+        <x:v>125930</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:3">
       <x:c r="A38" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C38" s="0" t="n">
-        <x:v>114453</x:v>
+        <x:v>122742</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:3">
       <x:c r="A39" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C39" s="0" t="n">
-        <x:v>111902</x:v>
+        <x:v>122742</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:3">
       <x:c r="A40" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C40" s="0" t="n">
-        <x:v>111584</x:v>
+        <x:v>120829</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:3">
       <x:c r="A41" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C41" s="0" t="n">
-        <x:v>111584</x:v>
+        <x:v>119554</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:3">
       <x:c r="A42" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C42" s="0" t="n">
-        <x:v>111265</x:v>
+        <x:v>119554</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:3">
       <x:c r="A43" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C43" s="0" t="n">
-        <x:v>111265</x:v>
+        <x:v>117957</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:3">
       <x:c r="A44" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C44" s="0" t="n">
-        <x:v>109989</x:v>
+        <x:v>114453</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:3">
       <x:c r="A45" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C45" s="0" t="n">
-        <x:v>108392</x:v>
+        <x:v>111902</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:3">
       <x:c r="A46" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C46" s="0" t="n">
-        <x:v>103613</x:v>
+        <x:v>111584</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:3">
       <x:c r="A47" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C47" s="0" t="n">
-        <x:v>102016</x:v>
+        <x:v>111584</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:3">
       <x:c r="A48" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C48" s="0" t="n">
-        <x:v>101700</x:v>
+        <x:v>111265</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:3">
       <x:c r="A49" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C49" s="0" t="n">
+        <x:v>111265</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:3">
+      <x:c r="A50" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="n">
+        <x:v>108392</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:3">
+      <x:c r="A51" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="n">
+        <x:v>103613</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:3">
+      <x:c r="A52" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="n">
+        <x:v>102016</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:3">
+      <x:c r="A53" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="n">
+        <x:v>101700</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:3">
+      <x:c r="A54" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="n">
         <x:v>100425</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:3">
+      <x:c r="A55" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="n">
+        <x:v>98831</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:3">
+      <x:c r="A56" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="n">
+        <x:v>98672</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:3">
+      <x:c r="A57" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="n">
+        <x:v>98512</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:3">
+      <x:c r="A58" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="n">
+        <x:v>95640</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:3">
+      <x:c r="A59" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="n">
+        <x:v>95324</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:3">
+      <x:c r="A60" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C60" s="0" t="n">
+        <x:v>92455</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:3">
+      <x:c r="A61" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C61" s="0" t="n">
+        <x:v>90861</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:3">
+      <x:c r="A62" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C62" s="0" t="n">
+        <x:v>87673</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>